<commit_message>
ajuste de nombre y correo electrónico
</commit_message>
<xml_diff>
--- a/Quiniela Semana 12 NFL 2025.xlsx
+++ b/Quiniela Semana 12 NFL 2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://citlali-my.sharepoint.com/personal/gaas_citlali_mx/Documents/Personal/Proyectos_personales/NFL/2025/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="11_C09132A136CC9A1BDE6008C81DE7A20E59B88AAB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F429DE5-E5B3-4222-94D8-93A7519CAA5E}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="11_C09132A136CC9A1BDE6008C81DE7A20E59B88AAB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D5759FF-1F1C-4FC1-A3C6-88F81A1AFF33}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -563,7 +563,7 @@
   <dimension ref="A1:P29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -636,7 +636,7 @@
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -1186,7 +1186,7 @@
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B13" t="s">
@@ -1386,7 +1386,7 @@
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B17" t="s">
@@ -1586,7 +1586,7 @@
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+      <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B21" t="s">
@@ -1941,7 +1941,7 @@
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+      <c r="A29" s="2" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>